<commit_message>
Atualizacao Tela de Lotes
</commit_message>
<xml_diff>
--- a/Tecnologia da Informação/Gráfico de Burndown.xlsx
+++ b/Tecnologia da Informação/Gráfico de Burndown.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27103"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,7 +15,7 @@
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -443,7 +443,7 @@
       <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>

</xml_diff>